<commit_message>
code Arduino/ fin semaine
Code Arduino:
-changement de couleur
-pression bouton
-récéption/envoi Serial
-Check connexion (souci: ne met pas en bleu à la déconnexion s'il n'y a pas de terminal)

Schema montage mis à jour mais ne l'est plus
</commit_message>
<xml_diff>
--- a/Doc/JournalTravail.xlsx
+++ b/Doc/JournalTravail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="83">
   <si>
     <t>Date</t>
   </si>
@@ -216,13 +216,94 @@
   </si>
   <si>
     <t>Légère modification du diagramme de code de l'application suite à la simplification due à l'API Skype.</t>
+  </si>
+  <si>
+    <t>Code Arduino</t>
+  </si>
+  <si>
+    <t>Je commence avec la partie communication du boitier. Mon module bluetooth a un pin STATE qui indique s'il est apairé ou non.</t>
+  </si>
+  <si>
+    <t>Il n'y a pas de patte sur ce pin, j'y soude un câble.</t>
+  </si>
+  <si>
+    <t>Création d'un code pour tester: c'est bon.</t>
+  </si>
+  <si>
+    <t>Test des LEDs et du bouton</t>
+  </si>
+  <si>
+    <t>Installation librairie neoPixel</t>
+  </si>
+  <si>
+    <t>https://learn.adafruit.com/adafruit-neopixel-uberguide/arduino-library-use</t>
+  </si>
+  <si>
+    <t>J'arrive à allumer les LEDs mais la couleur est différente sur chaque LED(devraient être toutes les mêmes), les deux dernières ne s'allument pas et deux d'entre elles changent de couleur au fil de l'éxecution.</t>
+  </si>
+  <si>
+    <r>
+      <t>J'ai une bande avec des pixels RGB</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>W</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> donc il faut indiquer ça à la création de l'objet contrôlant les LEDs.</t>
+    </r>
+  </si>
+  <si>
+    <t>Je regarde pour faire les interruptions. Il y a visiblement deux pins pour ça(2 et 3). Je vais mettre le bouton et STATE dessus. La loop gèrera la récéption Serial</t>
+  </si>
+  <si>
+    <t>Le bouton permet maintenant de passer à la couleur suivante mais ça change des fois quand le bouton descend, des fois quand il monte et des fois les deux. Lorsque le Bluetooth se connecte ou déconnecte, la couleur change.</t>
+  </si>
+  <si>
+    <t>Je regarde avec M.Ithurbide qui m'explique les rebonds du bouton. On va mettre un condo en // du bouton ainsi qu'utiliser un semaphore. Aussi il m'explique les machine à Etat.</t>
+  </si>
+  <si>
+    <t>Ajout du condo. Le souci est que ce montage avec le condensateur et la résistance pull-down inverse l'état.</t>
+  </si>
+  <si>
+    <t>En fait c'est parce que je mesure en //du bouton donc chute de tension de 5v dans le voltmètre. On pourrait mettre un filtre passe bas au lieu de mettre le condo en //.</t>
+  </si>
+  <si>
+    <t>Implémentation state machine, changement couleur, envoi de message au changement</t>
+  </si>
+  <si>
+    <t>Récéption Bluetooth: les messages seront soit pour changer la couleur (GREEN / RED / …) soit pour demander la présence (PING)</t>
+  </si>
+  <si>
+    <t>Je vais enlever mon interruption sur la fin du bluetooth car cela ne change finalement rien: si il n'y a plus de Bluetooth, il doit envoyer via USB. A la place, je vais périodiquement vérifier la présence de l'appli.</t>
+  </si>
+  <si>
+    <t>http://www.instructables.com/id/Arduino-Timer-Interrupts/</t>
+  </si>
+  <si>
+    <t>Mise en place interruption par timer et système check connection. Souci: le timeout change la couleur à bleu seulement s'il y a un terminal serial…</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -246,6 +327,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -261,7 +351,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -591,6 +681,41 @@
       <bottom style="double">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -598,7 +723,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -703,22 +828,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
@@ -727,19 +867,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1023,10 +1160,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A62" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A68" sqref="A68:D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1180,13 +1317,13 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A11" s="40">
+      <c r="A11" s="43">
         <v>43237</v>
       </c>
-      <c r="B11" s="37">
+      <c r="B11" s="41">
         <v>3.5</v>
       </c>
-      <c r="C11" s="37" t="s">
+      <c r="C11" s="41" t="s">
         <v>39</v>
       </c>
       <c r="D11" s="4" t="s">
@@ -1194,29 +1331,29 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="40"/>
-      <c r="B12" s="37"/>
-      <c r="C12" s="37"/>
+      <c r="A12" s="43"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="41"/>
       <c r="D12" s="30" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="45"/>
-      <c r="B13" s="44"/>
-      <c r="C13" s="44"/>
+      <c r="B13" s="46"/>
+      <c r="C13" s="46"/>
       <c r="D13" s="32" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="46">
+      <c r="A14" s="36">
         <v>43238</v>
       </c>
-      <c r="B14" s="47">
+      <c r="B14" s="38">
         <v>3.5</v>
       </c>
-      <c r="C14" s="47" t="s">
+      <c r="C14" s="38" t="s">
         <v>39</v>
       </c>
       <c r="D14" s="5" t="s">
@@ -1224,65 +1361,65 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="40"/>
-      <c r="B15" s="37"/>
-      <c r="C15" s="37"/>
+      <c r="A15" s="43"/>
+      <c r="B15" s="41"/>
+      <c r="C15" s="41"/>
       <c r="D15" s="30" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="40"/>
-      <c r="B16" s="37"/>
-      <c r="C16" s="37"/>
+      <c r="A16" s="43"/>
+      <c r="B16" s="41"/>
+      <c r="C16" s="41"/>
       <c r="D16" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="40"/>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
+      <c r="A17" s="43"/>
+      <c r="B17" s="41"/>
+      <c r="C17" s="41"/>
       <c r="D17" s="6" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="40"/>
-      <c r="B18" s="37"/>
-      <c r="C18" s="37"/>
+      <c r="A18" s="43"/>
+      <c r="B18" s="41"/>
+      <c r="C18" s="41"/>
       <c r="D18" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="40"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
+      <c r="A19" s="43"/>
+      <c r="B19" s="41"/>
+      <c r="C19" s="41"/>
       <c r="D19" s="6" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="40"/>
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
+      <c r="A20" s="43"/>
+      <c r="B20" s="41"/>
+      <c r="C20" s="41"/>
       <c r="D20" s="7" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="40"/>
-      <c r="B21" s="37"/>
-      <c r="C21" s="37"/>
+      <c r="A21" s="43"/>
+      <c r="B21" s="41"/>
+      <c r="C21" s="41"/>
       <c r="D21" s="7" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="41"/>
-      <c r="B22" s="38"/>
-      <c r="C22" s="38"/>
+      <c r="A22" s="37"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="39"/>
       <c r="D22" s="8" t="s">
         <v>30</v>
       </c>
@@ -1302,13 +1439,13 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="40">
+      <c r="A24" s="43">
         <v>43242</v>
       </c>
-      <c r="B24" s="37">
+      <c r="B24" s="41">
         <v>1</v>
       </c>
-      <c r="C24" s="37" t="s">
+      <c r="C24" s="41" t="s">
         <v>29</v>
       </c>
       <c r="D24" s="2" t="s">
@@ -1316,25 +1453,25 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="40"/>
-      <c r="B25" s="37"/>
-      <c r="C25" s="37"/>
+      <c r="A25" s="43"/>
+      <c r="B25" s="41"/>
+      <c r="C25" s="41"/>
       <c r="D25" s="31" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="40"/>
-      <c r="B26" s="37"/>
-      <c r="C26" s="42"/>
+      <c r="A26" s="43"/>
+      <c r="B26" s="41"/>
+      <c r="C26" s="47"/>
       <c r="D26" s="4" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A27" s="41"/>
-      <c r="B27" s="38"/>
-      <c r="C27" s="43"/>
+      <c r="A27" s="37"/>
+      <c r="B27" s="39"/>
+      <c r="C27" s="48"/>
       <c r="D27" s="8" t="s">
         <v>38</v>
       </c>
@@ -1354,13 +1491,13 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="39">
+      <c r="A29" s="42">
         <v>43242</v>
       </c>
-      <c r="B29" s="36">
+      <c r="B29" s="40">
         <v>1</v>
       </c>
-      <c r="C29" s="36" t="s">
+      <c r="C29" s="40" t="s">
         <v>39</v>
       </c>
       <c r="D29" s="29" t="s">
@@ -1368,21 +1505,21 @@
       </c>
     </row>
     <row r="30" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="48"/>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
+      <c r="A30" s="44"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
       <c r="D30" s="8" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="39">
+      <c r="A31" s="42">
         <v>43242</v>
       </c>
-      <c r="B31" s="36">
+      <c r="B31" s="40">
         <v>2</v>
       </c>
-      <c r="C31" s="36" t="s">
+      <c r="C31" s="40" t="s">
         <v>29</v>
       </c>
       <c r="D31" s="28" t="s">
@@ -1391,20 +1528,20 @@
     </row>
     <row r="32" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="45"/>
-      <c r="B32" s="44"/>
-      <c r="C32" s="44"/>
+      <c r="B32" s="46"/>
+      <c r="C32" s="46"/>
       <c r="D32" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="46">
+      <c r="A33" s="36">
         <v>43243</v>
       </c>
-      <c r="B33" s="47">
+      <c r="B33" s="38">
         <v>1</v>
       </c>
-      <c r="C33" s="47" t="s">
+      <c r="C33" s="38" t="s">
         <v>8</v>
       </c>
       <c r="D33" s="5" t="s">
@@ -1412,9 +1549,9 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="41"/>
-      <c r="B34" s="38"/>
-      <c r="C34" s="38"/>
+      <c r="A34" s="37"/>
+      <c r="B34" s="39"/>
+      <c r="C34" s="39"/>
       <c r="D34" s="8" t="s">
         <v>44</v>
       </c>
@@ -1434,13 +1571,13 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A36" s="39">
+      <c r="A36" s="42">
         <v>43243</v>
       </c>
-      <c r="B36" s="36">
+      <c r="B36" s="40">
         <v>1.5</v>
       </c>
-      <c r="C36" s="36" t="s">
+      <c r="C36" s="40" t="s">
         <v>14</v>
       </c>
       <c r="D36" s="28" t="s">
@@ -1448,45 +1585,45 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="40"/>
-      <c r="B37" s="37"/>
-      <c r="C37" s="37"/>
+      <c r="A37" s="43"/>
+      <c r="B37" s="41"/>
+      <c r="C37" s="41"/>
       <c r="D37" s="30" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="40"/>
-      <c r="B38" s="37"/>
-      <c r="C38" s="37"/>
+      <c r="A38" s="43"/>
+      <c r="B38" s="41"/>
+      <c r="C38" s="41"/>
       <c r="D38" s="4" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="40"/>
-      <c r="B39" s="37"/>
-      <c r="C39" s="37"/>
+      <c r="A39" s="43"/>
+      <c r="B39" s="41"/>
+      <c r="C39" s="41"/>
       <c r="D39" s="30" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" s="41"/>
-      <c r="B40" s="38"/>
-      <c r="C40" s="38"/>
+      <c r="A40" s="37"/>
+      <c r="B40" s="39"/>
+      <c r="C40" s="39"/>
       <c r="D40" s="8" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="39">
+      <c r="A41" s="42">
         <v>43243</v>
       </c>
-      <c r="B41" s="36">
+      <c r="B41" s="40">
         <v>1</v>
       </c>
-      <c r="C41" s="36" t="s">
+      <c r="C41" s="40" t="s">
         <v>29</v>
       </c>
       <c r="D41" s="28" t="s">
@@ -1494,29 +1631,29 @@
       </c>
     </row>
     <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="40"/>
-      <c r="B42" s="37"/>
-      <c r="C42" s="37"/>
+      <c r="A42" s="43"/>
+      <c r="B42" s="41"/>
+      <c r="C42" s="41"/>
       <c r="D42" s="4" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="41"/>
-      <c r="B43" s="38"/>
-      <c r="C43" s="38"/>
+      <c r="A43" s="37"/>
+      <c r="B43" s="39"/>
+      <c r="C43" s="39"/>
       <c r="D43" s="33" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="39">
+      <c r="A44" s="42">
         <v>43243</v>
       </c>
-      <c r="B44" s="36">
+      <c r="B44" s="40">
         <v>2</v>
       </c>
-      <c r="C44" s="36" t="s">
+      <c r="C44" s="40" t="s">
         <v>39</v>
       </c>
       <c r="D44" s="34" t="s">
@@ -1524,41 +1661,41 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A45" s="40"/>
-      <c r="B45" s="37"/>
-      <c r="C45" s="37"/>
+      <c r="A45" s="43"/>
+      <c r="B45" s="41"/>
+      <c r="C45" s="41"/>
       <c r="D45" s="4" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A46" s="40"/>
-      <c r="B46" s="37"/>
-      <c r="C46" s="37"/>
+      <c r="A46" s="43"/>
+      <c r="B46" s="41"/>
+      <c r="C46" s="41"/>
       <c r="D46" s="4" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A47" s="40"/>
-      <c r="B47" s="37"/>
-      <c r="C47" s="37"/>
+      <c r="A47" s="43"/>
+      <c r="B47" s="41"/>
+      <c r="C47" s="41"/>
       <c r="D47" s="4" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A48" s="40"/>
-      <c r="B48" s="37"/>
-      <c r="C48" s="37"/>
+      <c r="A48" s="43"/>
+      <c r="B48" s="41"/>
+      <c r="C48" s="41"/>
       <c r="D48" s="30" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A49" s="41"/>
-      <c r="B49" s="38"/>
-      <c r="C49" s="38"/>
+      <c r="A49" s="37"/>
+      <c r="B49" s="39"/>
+      <c r="C49" s="39"/>
       <c r="D49" s="8" t="s">
         <v>59</v>
       </c>
@@ -1591,20 +1728,222 @@
         <v>63</v>
       </c>
     </row>
+    <row r="52" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A52" s="42">
+        <v>43244</v>
+      </c>
+      <c r="B52" s="40">
+        <v>2</v>
+      </c>
+      <c r="C52" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="D52" s="49" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="43"/>
+      <c r="B53" s="41"/>
+      <c r="C53" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="D53" s="49" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="37"/>
+      <c r="B54" s="39"/>
+      <c r="C54" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="D54" s="50" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="42">
+        <v>43244</v>
+      </c>
+      <c r="B55" s="40">
+        <v>2</v>
+      </c>
+      <c r="C55" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="D55" s="28" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="43"/>
+      <c r="B56" s="41"/>
+      <c r="C56" s="41"/>
+      <c r="D56" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="43"/>
+      <c r="B57" s="41"/>
+      <c r="C57" s="41"/>
+      <c r="D57" s="30" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A58" s="43"/>
+      <c r="B58" s="41"/>
+      <c r="C58" s="41"/>
+      <c r="D58" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="37"/>
+      <c r="B59" s="39"/>
+      <c r="C59" s="39"/>
+      <c r="D59" s="51" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A60" s="42">
+        <v>43244</v>
+      </c>
+      <c r="B60" s="40">
+        <v>1.5</v>
+      </c>
+      <c r="C60" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A61" s="37"/>
+      <c r="B61" s="39"/>
+      <c r="C61" s="39"/>
+      <c r="D61" s="51" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="20">
+        <v>43244</v>
+      </c>
+      <c r="B62" s="21">
+        <v>1</v>
+      </c>
+      <c r="C62" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D62" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="36">
+        <v>43245</v>
+      </c>
+      <c r="B63" s="38">
+        <v>1.5</v>
+      </c>
+      <c r="C63" s="52" t="s">
+        <v>61</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A64" s="37"/>
+      <c r="B64" s="39"/>
+      <c r="C64" s="48"/>
+      <c r="D64" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="42">
+        <v>43245</v>
+      </c>
+      <c r="B65" s="40">
+        <v>2</v>
+      </c>
+      <c r="C65" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="D65" s="28" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A66" s="43"/>
+      <c r="B66" s="41"/>
+      <c r="C66" s="41"/>
+      <c r="D66" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A67" s="37"/>
+      <c r="B67" s="39"/>
+      <c r="C67" s="39"/>
+      <c r="D67" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="42">
+        <v>43245</v>
+      </c>
+      <c r="B68" s="40">
+        <v>1.5</v>
+      </c>
+      <c r="C68" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="D68" s="28" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="45"/>
+      <c r="B69" s="46"/>
+      <c r="C69" s="46"/>
+      <c r="D69" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="C36:C40"/>
-    <mergeCell ref="B36:B40"/>
-    <mergeCell ref="A36:A40"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C31:C32"/>
+  <mergeCells count="44">
+    <mergeCell ref="A68:A69"/>
+    <mergeCell ref="B68:B69"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="C65:C67"/>
+    <mergeCell ref="B65:B67"/>
+    <mergeCell ref="A65:A67"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="B52:B54"/>
+    <mergeCell ref="A52:A54"/>
+    <mergeCell ref="A55:A59"/>
+    <mergeCell ref="B55:B59"/>
+    <mergeCell ref="C55:C59"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="A44:A49"/>
+    <mergeCell ref="B44:B49"/>
+    <mergeCell ref="C44:C49"/>
     <mergeCell ref="A24:A27"/>
     <mergeCell ref="B24:B27"/>
     <mergeCell ref="C24:C27"/>
@@ -1614,12 +1953,18 @@
     <mergeCell ref="A14:A22"/>
     <mergeCell ref="B14:B22"/>
     <mergeCell ref="C14:C22"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="A44:A49"/>
-    <mergeCell ref="B44:B49"/>
-    <mergeCell ref="C44:C49"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="C36:C40"/>
+    <mergeCell ref="B36:B40"/>
+    <mergeCell ref="A36:A40"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D29" r:id="rId1"/>
@@ -1631,9 +1976,10 @@
     <hyperlink ref="D12" r:id="rId7"/>
     <hyperlink ref="D43" r:id="rId8"/>
     <hyperlink ref="D48" r:id="rId9"/>
+    <hyperlink ref="D57" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"-,Gras"Présentiel pour open space&amp;C&amp;"-,Gras"&amp;14Journal de travail&amp;R&amp;"-,Gras"Cyril Kalbfuss</oddHeader>
   </headerFooter>

</xml_diff>

<commit_message>
App-Skype et switch mode communication
Application:
-Skype fonctionnel
-Bouton switch USB/Bluetooth
-Fix: Thread serial ne peut envoyer qu'un message à la fois cause omisssions.
</commit_message>
<xml_diff>
--- a/Doc/JournalTravail.xlsx
+++ b/Doc/JournalTravail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="111">
   <si>
     <t>Date</t>
   </si>
@@ -333,6 +333,54 @@
   </si>
   <si>
     <t>Il faut maintenant gérer les évènements de skype pour pouvoir modifier les éléments UI en rapport.</t>
+  </si>
+  <si>
+    <t>Ajout des évènements de synchronisation entre le thread de skype et celui de l'UI. Si Skype n'est pas lancé, impossible d'avoir le Client. Dans ce cas il faudra vérifier périodiquement. De plus lorsque Skype est quitté sans fair signOut, cela provoque aussi un crash.</t>
+  </si>
+  <si>
+    <t>Ajout des mesures pour la détéction de connexion skype et le lancement de skype en cours d'exécution</t>
+  </si>
+  <si>
+    <t>Il y a un souci du côté de l'arduino. Après quelques tests, il arrive que plusieurs lignes arrivent trop proche et qu'il les prenne comme une seule. Je vais devoir gérer ça.</t>
+  </si>
+  <si>
+    <t>Correction du souci multiligne</t>
+  </si>
+  <si>
+    <t>Mise à jour de la présence skype lorsqu'appui sur le bouton</t>
+  </si>
+  <si>
+    <t>https://blog.thoughtstuff.co.uk/2016/06/skypedevq-updating-skype-for-business-presence-client-sdk/</t>
+  </si>
+  <si>
+    <t>Test App</t>
+  </si>
+  <si>
+    <t>il reste des soucis de synchronisation lorsqu'il y a une reconnexion de skype. (Skype est déconnecté en cours d'exécution puis reconnecté, ça ne met plus à jour de l'app au boitier)</t>
+  </si>
+  <si>
+    <t>Lorsque Skype est reconnecté, les evènements pour l'activité ne se déclenchent plu. Ceux pour la connexion par contre, si. Si je quitte complètement Skype et relance, plus rien n'est capté. Il faut donc que je recréer l'objet lorsque Skype quitte et qui je refasse l'event lorsque skype se reconnecte.</t>
+  </si>
+  <si>
+    <t>Pour la reconnexion: simple il suffit de reset un de mes flags à signout. Pour le cas ou le programme quitte, cela ne lance pas l'état "shutting down". J'utilise l'évènement ClientDisconnected disponible pour les objetc LyncClient mais pas Client. Je change donc le type de mon objet client.</t>
+  </si>
+  <si>
+    <t>Observation</t>
+  </si>
+  <si>
+    <t>Analyse à l'oscilloscope des appui de boutons avec et sans filtre</t>
+  </si>
+  <si>
+    <t>Problème suivant: lors du lancement de l'app , le boitier ne chanche pas sa couleur. Le problème vient du fait qu'il y a deux "send" très proche et la fonction que j'ai fait n'en permet qu'un à la fois. Je vais mettre une liste au lieu d'une seule String</t>
+  </si>
+  <si>
+    <t>Ajout d'images logo usb et bluetooth en tant que resources et création d'un bouton pour le switch usb/bluetooth.</t>
+  </si>
+  <si>
+    <t>Code switch sur appui du bouton. Souci: on ne peut pas revenir sur le mode précédent. Le port est occupé.</t>
+  </si>
+  <si>
+    <t>Revue partie conception matérielle. Préparation du rendu et synchronisation github.</t>
   </si>
 </sst>
 </file>
@@ -759,7 +807,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -792,51 +840,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -873,82 +897,112 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1232,28 +1286,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F81"/>
+  <dimension ref="A1:F95"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C83" sqref="C83"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A91" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B97" sqref="B97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" style="22" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" style="23" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" style="23" customWidth="1"/>
+    <col min="1" max="1" width="10" style="66" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" style="31" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="17" customWidth="1"/>
     <col min="4" max="4" width="52" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="10" t="s">
@@ -1263,13 +1317,13 @@
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="14">
+      <c r="A2" s="33">
         <v>43235</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="34">
         <v>1</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="13" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="8" t="s">
@@ -1277,13 +1331,13 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="14">
+      <c r="A3" s="33">
         <v>43235</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="34">
         <v>1.5</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="13" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="8" t="s">
@@ -1291,13 +1345,13 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="16">
+      <c r="A4" s="37">
         <v>43235</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="38">
         <v>1.5</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="14" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -1305,13 +1359,13 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="18">
+      <c r="A5" s="62">
         <v>43236</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="59">
         <v>0.5</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="15" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="9" t="s">
@@ -1319,13 +1373,13 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="14">
+      <c r="A6" s="33">
         <v>43236</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="34">
         <v>2</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="13" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="8" t="s">
@@ -1333,13 +1387,13 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="14">
+      <c r="A7" s="33">
         <v>43236</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="34">
         <v>2</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="13" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="8" t="s">
@@ -1347,13 +1401,13 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="16">
+      <c r="A8" s="37">
         <v>43236</v>
       </c>
-      <c r="B8" s="17">
+      <c r="B8" s="38">
         <v>2.5</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="14" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -1361,13 +1415,13 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="18">
+      <c r="A9" s="62">
         <v>43237</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B9" s="59">
         <v>1</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="15" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="9" t="s">
@@ -1375,13 +1429,13 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="14">
+      <c r="A10" s="33">
         <v>43237</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B10" s="34">
         <v>2.5</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="13" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="8" t="s">
@@ -1389,13 +1443,13 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A11" s="50">
+      <c r="A11" s="43">
         <v>43237</v>
       </c>
-      <c r="B11" s="49">
+      <c r="B11" s="40">
         <v>3.5</v>
       </c>
-      <c r="C11" s="49" t="s">
+      <c r="C11" s="52" t="s">
         <v>39</v>
       </c>
       <c r="D11" s="4" t="s">
@@ -1403,18 +1457,18 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="50"/>
-      <c r="B12" s="49"/>
-      <c r="C12" s="49"/>
-      <c r="D12" s="30" t="s">
+      <c r="A12" s="43"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="22" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="40"/>
-      <c r="B13" s="42"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="32" t="s">
+      <c r="A13" s="44"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="24" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1425,7 +1479,7 @@
       <c r="B14" s="45">
         <v>3.5</v>
       </c>
-      <c r="C14" s="45" t="s">
+      <c r="C14" s="49" t="s">
         <v>39</v>
       </c>
       <c r="D14" s="5" t="s">
@@ -1433,57 +1487,57 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="50"/>
-      <c r="B15" s="49"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="30" t="s">
+      <c r="A15" s="43"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="22" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="50"/>
-      <c r="B16" s="49"/>
-      <c r="C16" s="49"/>
+      <c r="A16" s="43"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="52"/>
       <c r="D16" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="50"/>
-      <c r="B17" s="49"/>
-      <c r="C17" s="49"/>
+      <c r="A17" s="43"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="52"/>
       <c r="D17" s="6" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="50"/>
-      <c r="B18" s="49"/>
-      <c r="C18" s="49"/>
+      <c r="A18" s="43"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="52"/>
       <c r="D18" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="50"/>
-      <c r="B19" s="49"/>
-      <c r="C19" s="49"/>
+      <c r="A19" s="43"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="52"/>
       <c r="D19" s="6" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="50"/>
-      <c r="B20" s="49"/>
-      <c r="C20" s="49"/>
+      <c r="A20" s="43"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="52"/>
       <c r="D20" s="7" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="50"/>
-      <c r="B21" s="49"/>
-      <c r="C21" s="49"/>
+      <c r="A21" s="43"/>
+      <c r="B21" s="40"/>
+      <c r="C21" s="52"/>
       <c r="D21" s="7" t="s">
         <v>27</v>
       </c>
@@ -1491,19 +1545,19 @@
     <row r="22" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="48"/>
       <c r="B22" s="46"/>
-      <c r="C22" s="46"/>
+      <c r="C22" s="50"/>
       <c r="D22" s="8" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="20">
+      <c r="A23" s="63">
         <v>43238</v>
       </c>
-      <c r="B23" s="21">
+      <c r="B23" s="60">
         <v>2</v>
       </c>
-      <c r="C23" s="21" t="s">
+      <c r="C23" s="16" t="s">
         <v>29</v>
       </c>
       <c r="D23" s="11" t="s">
@@ -1511,13 +1565,13 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="50">
+      <c r="A24" s="43">
         <v>43242</v>
       </c>
-      <c r="B24" s="49">
+      <c r="B24" s="40">
         <v>1</v>
       </c>
-      <c r="C24" s="49" t="s">
+      <c r="C24" s="52" t="s">
         <v>29</v>
       </c>
       <c r="D24" s="2" t="s">
@@ -1525,17 +1579,17 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="50"/>
-      <c r="B25" s="49"/>
-      <c r="C25" s="49"/>
-      <c r="D25" s="31" t="s">
+      <c r="A25" s="43"/>
+      <c r="B25" s="40"/>
+      <c r="C25" s="52"/>
+      <c r="D25" s="23" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="50"/>
-      <c r="B26" s="49"/>
-      <c r="C26" s="51"/>
+      <c r="A26" s="43"/>
+      <c r="B26" s="40"/>
+      <c r="C26" s="54"/>
       <c r="D26" s="4" t="s">
         <v>33</v>
       </c>
@@ -1543,19 +1597,19 @@
     <row r="27" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="48"/>
       <c r="B27" s="46"/>
-      <c r="C27" s="44"/>
+      <c r="C27" s="55"/>
       <c r="D27" s="8" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A28" s="24">
+      <c r="A28" s="64">
         <v>43242</v>
       </c>
-      <c r="B28" s="25">
+      <c r="B28" s="57">
         <v>0</v>
       </c>
-      <c r="C28" s="25" t="s">
+      <c r="C28" s="18" t="s">
         <v>34</v>
       </c>
       <c r="D28" s="8" t="s">
@@ -1563,45 +1617,45 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="39">
+      <c r="A29" s="42">
         <v>43242</v>
       </c>
-      <c r="B29" s="41">
+      <c r="B29" s="39">
         <v>1</v>
       </c>
-      <c r="C29" s="41" t="s">
+      <c r="C29" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="D29" s="29" t="s">
+      <c r="D29" s="21" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="52"/>
+      <c r="A30" s="65"/>
       <c r="B30" s="46"/>
-      <c r="C30" s="46"/>
+      <c r="C30" s="50"/>
       <c r="D30" s="8" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="39">
+      <c r="A31" s="42">
         <v>43242</v>
       </c>
-      <c r="B31" s="41">
+      <c r="B31" s="39">
         <v>2</v>
       </c>
-      <c r="C31" s="41" t="s">
+      <c r="C31" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="D31" s="28" t="s">
+      <c r="D31" s="20" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="40"/>
-      <c r="B32" s="42"/>
-      <c r="C32" s="42"/>
+      <c r="A32" s="44"/>
+      <c r="B32" s="41"/>
+      <c r="C32" s="53"/>
       <c r="D32" s="3" t="s">
         <v>42</v>
       </c>
@@ -1613,7 +1667,7 @@
       <c r="B33" s="45">
         <v>1</v>
       </c>
-      <c r="C33" s="45" t="s">
+      <c r="C33" s="49" t="s">
         <v>8</v>
       </c>
       <c r="D33" s="5" t="s">
@@ -1623,19 +1677,19 @@
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="48"/>
       <c r="B34" s="46"/>
-      <c r="C34" s="46"/>
+      <c r="C34" s="50"/>
       <c r="D34" s="8" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="26">
+      <c r="A35" s="32">
         <v>43243</v>
       </c>
-      <c r="B35" s="27">
+      <c r="B35" s="31">
         <v>0.5</v>
       </c>
-      <c r="C35" s="27" t="s">
+      <c r="C35" s="19" t="s">
         <v>50</v>
       </c>
       <c r="D35" s="4" t="s">
@@ -1643,69 +1697,69 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A36" s="39">
+      <c r="A36" s="42">
         <v>43243</v>
       </c>
-      <c r="B36" s="41">
+      <c r="B36" s="39">
         <v>1.5</v>
       </c>
-      <c r="C36" s="41" t="s">
+      <c r="C36" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="D36" s="28" t="s">
+      <c r="D36" s="20" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="50"/>
-      <c r="B37" s="49"/>
-      <c r="C37" s="49"/>
-      <c r="D37" s="30" t="s">
+      <c r="A37" s="43"/>
+      <c r="B37" s="40"/>
+      <c r="C37" s="52"/>
+      <c r="D37" s="22" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="50"/>
-      <c r="B38" s="49"/>
-      <c r="C38" s="49"/>
+      <c r="A38" s="43"/>
+      <c r="B38" s="40"/>
+      <c r="C38" s="52"/>
       <c r="D38" s="4" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="50"/>
-      <c r="B39" s="49"/>
-      <c r="C39" s="49"/>
-      <c r="D39" s="30" t="s">
+      <c r="A39" s="43"/>
+      <c r="B39" s="40"/>
+      <c r="C39" s="52"/>
+      <c r="D39" s="22" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="48"/>
       <c r="B40" s="46"/>
-      <c r="C40" s="46"/>
+      <c r="C40" s="50"/>
       <c r="D40" s="8" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="39">
+      <c r="A41" s="42">
         <v>43243</v>
       </c>
-      <c r="B41" s="41">
+      <c r="B41" s="39">
         <v>1</v>
       </c>
-      <c r="C41" s="41" t="s">
+      <c r="C41" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="D41" s="28" t="s">
+      <c r="D41" s="20" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="50"/>
-      <c r="B42" s="49"/>
-      <c r="C42" s="49"/>
+      <c r="A42" s="43"/>
+      <c r="B42" s="40"/>
+      <c r="C42" s="52"/>
       <c r="D42" s="4" t="s">
         <v>54</v>
       </c>
@@ -1713,87 +1767,87 @@
     <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="48"/>
       <c r="B43" s="46"/>
-      <c r="C43" s="46"/>
-      <c r="D43" s="33" t="s">
+      <c r="C43" s="50"/>
+      <c r="D43" s="25" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="39">
+      <c r="A44" s="42">
         <v>43243</v>
       </c>
-      <c r="B44" s="41">
+      <c r="B44" s="39">
         <v>2</v>
       </c>
-      <c r="C44" s="41" t="s">
+      <c r="C44" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="D44" s="34" t="s">
+      <c r="D44" s="26" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A45" s="50"/>
-      <c r="B45" s="49"/>
-      <c r="C45" s="49"/>
+      <c r="A45" s="43"/>
+      <c r="B45" s="40"/>
+      <c r="C45" s="52"/>
       <c r="D45" s="4" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A46" s="50"/>
-      <c r="B46" s="49"/>
-      <c r="C46" s="49"/>
+      <c r="A46" s="43"/>
+      <c r="B46" s="40"/>
+      <c r="C46" s="52"/>
       <c r="D46" s="4" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A47" s="50"/>
-      <c r="B47" s="49"/>
-      <c r="C47" s="49"/>
+      <c r="A47" s="43"/>
+      <c r="B47" s="40"/>
+      <c r="C47" s="52"/>
       <c r="D47" s="4" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A48" s="50"/>
-      <c r="B48" s="49"/>
-      <c r="C48" s="49"/>
-      <c r="D48" s="30" t="s">
+      <c r="A48" s="43"/>
+      <c r="B48" s="40"/>
+      <c r="C48" s="52"/>
+      <c r="D48" s="22" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" s="48"/>
       <c r="B49" s="46"/>
-      <c r="C49" s="46"/>
+      <c r="C49" s="50"/>
       <c r="D49" s="8" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="20">
+      <c r="A50" s="63">
         <v>43243</v>
       </c>
-      <c r="B50" s="21">
+      <c r="B50" s="60">
         <v>1</v>
       </c>
-      <c r="C50" s="21" t="s">
+      <c r="C50" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="D50" s="35" t="s">
+      <c r="D50" s="27" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="18">
+      <c r="A51" s="62">
         <v>43244</v>
       </c>
-      <c r="B51" s="19">
+      <c r="B51" s="59">
         <v>0.5</v>
       </c>
-      <c r="C51" s="19" t="s">
+      <c r="C51" s="15" t="s">
         <v>14</v>
       </c>
       <c r="D51" s="9" t="s">
@@ -1801,73 +1855,73 @@
       </c>
     </row>
     <row r="52" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A52" s="39">
+      <c r="A52" s="42">
         <v>43244</v>
       </c>
-      <c r="B52" s="41">
+      <c r="B52" s="39">
         <v>2</v>
       </c>
-      <c r="C52" s="25" t="s">
+      <c r="C52" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="D52" s="36" t="s">
+      <c r="D52" s="28" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="50"/>
-      <c r="B53" s="49"/>
-      <c r="C53" s="25" t="s">
+      <c r="A53" s="43"/>
+      <c r="B53" s="40"/>
+      <c r="C53" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="D53" s="36" t="s">
+      <c r="D53" s="28" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="48"/>
       <c r="B54" s="46"/>
-      <c r="C54" s="25" t="s">
+      <c r="C54" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="D54" s="37" t="s">
+      <c r="D54" s="29" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="39">
+      <c r="A55" s="42">
         <v>43244</v>
       </c>
-      <c r="B55" s="41">
+      <c r="B55" s="39">
         <v>2</v>
       </c>
-      <c r="C55" s="41" t="s">
+      <c r="C55" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="D55" s="28" t="s">
+      <c r="D55" s="20" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="50"/>
-      <c r="B56" s="49"/>
-      <c r="C56" s="49"/>
+      <c r="A56" s="43"/>
+      <c r="B56" s="40"/>
+      <c r="C56" s="52"/>
       <c r="D56" s="4" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="50"/>
-      <c r="B57" s="49"/>
-      <c r="C57" s="49"/>
-      <c r="D57" s="30" t="s">
+      <c r="A57" s="43"/>
+      <c r="B57" s="40"/>
+      <c r="C57" s="52"/>
+      <c r="D57" s="22" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A58" s="50"/>
-      <c r="B58" s="49"/>
-      <c r="C58" s="49"/>
+      <c r="A58" s="43"/>
+      <c r="B58" s="40"/>
+      <c r="C58" s="52"/>
       <c r="D58" s="4" t="s">
         <v>71</v>
       </c>
@@ -1875,19 +1929,19 @@
     <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="48"/>
       <c r="B59" s="46"/>
-      <c r="C59" s="46"/>
-      <c r="D59" s="38" t="s">
+      <c r="C59" s="50"/>
+      <c r="D59" s="30" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A60" s="39">
+      <c r="A60" s="42">
         <v>43244</v>
       </c>
-      <c r="B60" s="41">
+      <c r="B60" s="39">
         <v>1.5</v>
       </c>
-      <c r="C60" s="41" t="s">
+      <c r="C60" s="51" t="s">
         <v>64</v>
       </c>
       <c r="D60" s="2" t="s">
@@ -1897,19 +1951,19 @@
     <row r="61" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A61" s="48"/>
       <c r="B61" s="46"/>
-      <c r="C61" s="46"/>
-      <c r="D61" s="38" t="s">
+      <c r="C61" s="50"/>
+      <c r="D61" s="30" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="20">
+      <c r="A62" s="63">
         <v>43244</v>
       </c>
-      <c r="B62" s="21">
+      <c r="B62" s="60">
         <v>1</v>
       </c>
-      <c r="C62" s="21" t="s">
+      <c r="C62" s="16" t="s">
         <v>8</v>
       </c>
       <c r="D62" s="11" t="s">
@@ -1923,7 +1977,7 @@
       <c r="B63" s="45">
         <v>1.5</v>
       </c>
-      <c r="C63" s="43" t="s">
+      <c r="C63" s="56" t="s">
         <v>61</v>
       </c>
       <c r="D63" s="4" t="s">
@@ -1933,29 +1987,29 @@
     <row r="64" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A64" s="48"/>
       <c r="B64" s="46"/>
-      <c r="C64" s="44"/>
+      <c r="C64" s="55"/>
       <c r="D64" s="8" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A65" s="39">
+      <c r="A65" s="42">
         <v>43245</v>
       </c>
-      <c r="B65" s="41">
+      <c r="B65" s="39">
         <v>2</v>
       </c>
-      <c r="C65" s="41" t="s">
+      <c r="C65" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="D65" s="28" t="s">
+      <c r="D65" s="20" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A66" s="50"/>
-      <c r="B66" s="49"/>
-      <c r="C66" s="49"/>
+      <c r="A66" s="43"/>
+      <c r="B66" s="40"/>
+      <c r="C66" s="52"/>
       <c r="D66" s="4" t="s">
         <v>80</v>
       </c>
@@ -1963,41 +2017,41 @@
     <row r="67" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" s="48"/>
       <c r="B67" s="46"/>
-      <c r="C67" s="46"/>
+      <c r="C67" s="50"/>
       <c r="D67" s="8" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="39">
+      <c r="A68" s="42">
         <v>43245</v>
       </c>
-      <c r="B68" s="41">
+      <c r="B68" s="39">
         <v>1.5</v>
       </c>
-      <c r="C68" s="41" t="s">
+      <c r="C68" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="D68" s="29" t="s">
+      <c r="D68" s="21" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="40"/>
-      <c r="B69" s="42"/>
-      <c r="C69" s="42"/>
+      <c r="A69" s="44"/>
+      <c r="B69" s="41"/>
+      <c r="C69" s="53"/>
       <c r="D69" s="3" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="18">
+      <c r="A70" s="62">
         <v>43249</v>
       </c>
-      <c r="B70" s="19">
+      <c r="B70" s="59">
         <v>1</v>
       </c>
-      <c r="C70" s="19" t="s">
+      <c r="C70" s="15" t="s">
         <v>83</v>
       </c>
       <c r="D70" s="9" t="s">
@@ -2005,41 +2059,41 @@
       </c>
     </row>
     <row r="71" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A71" s="24">
+      <c r="A71" s="64">
         <v>43249</v>
       </c>
-      <c r="B71" s="25">
+      <c r="B71" s="57">
         <v>1</v>
       </c>
-      <c r="C71" s="25" t="s">
+      <c r="C71" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="D71" s="36" t="s">
+      <c r="D71" s="28" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="20">
+      <c r="A72" s="63">
         <v>43249</v>
       </c>
-      <c r="B72" s="21">
+      <c r="B72" s="60">
         <v>1.5</v>
       </c>
-      <c r="C72" s="21" t="s">
+      <c r="C72" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="D72" s="35" t="s">
+      <c r="D72" s="27" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="55">
+      <c r="A73" s="47">
         <v>43250</v>
       </c>
-      <c r="B73" s="53">
+      <c r="B73" s="45">
         <v>2</v>
       </c>
-      <c r="C73" s="53" t="s">
+      <c r="C73" s="45" t="s">
         <v>83</v>
       </c>
       <c r="D73" s="5" t="s">
@@ -2047,76 +2101,295 @@
       </c>
     </row>
     <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="57"/>
-      <c r="B74" s="58"/>
-      <c r="C74" s="58"/>
-      <c r="D74" s="33" t="s">
+      <c r="A74" s="48"/>
+      <c r="B74" s="46"/>
+      <c r="C74" s="46"/>
+      <c r="D74" s="25" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A75" s="59">
+      <c r="A75" s="42">
         <v>43250</v>
       </c>
-      <c r="B75" s="60">
+      <c r="B75" s="39">
         <v>1.5</v>
       </c>
-      <c r="C75" s="60" t="s">
+      <c r="C75" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="D75" s="61" t="s">
+      <c r="D75" s="35" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A76" s="57"/>
-      <c r="B76" s="58"/>
-      <c r="C76" s="58"/>
-      <c r="D76" s="62" t="s">
+      <c r="A76" s="48"/>
+      <c r="B76" s="46"/>
+      <c r="C76" s="46"/>
+      <c r="D76" s="36" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A77" s="59">
+      <c r="A77" s="42">
         <v>43250</v>
       </c>
-      <c r="B77" s="60">
+      <c r="B77" s="39">
         <v>0.5</v>
       </c>
-      <c r="C77" s="60" t="s">
+      <c r="C77" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="D77" s="28" t="s">
+      <c r="D77" s="20" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="56"/>
-      <c r="B78" s="54"/>
-      <c r="C78" s="54"/>
+      <c r="A78" s="43"/>
+      <c r="B78" s="40"/>
+      <c r="C78" s="40"/>
       <c r="D78" s="4" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A79" s="56"/>
-      <c r="B79" s="54"/>
-      <c r="C79" s="54"/>
+      <c r="A79" s="43"/>
+      <c r="B79" s="40"/>
+      <c r="C79" s="40"/>
       <c r="D79" s="4" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="63"/>
-      <c r="B80" s="64"/>
-      <c r="C80" s="64"/>
+      <c r="A80" s="44"/>
+      <c r="B80" s="41"/>
+      <c r="C80" s="41"/>
       <c r="D80" s="3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="81" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="81" spans="1:4" ht="75.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="47">
+        <v>43251</v>
+      </c>
+      <c r="B81" s="45">
+        <v>4</v>
+      </c>
+      <c r="C81" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A82" s="43"/>
+      <c r="B82" s="40"/>
+      <c r="C82" s="40"/>
+      <c r="D82" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A83" s="48"/>
+      <c r="B83" s="46"/>
+      <c r="C83" s="46"/>
+      <c r="D83" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="64">
+        <v>43251</v>
+      </c>
+      <c r="B84" s="57">
+        <v>1</v>
+      </c>
+      <c r="C84" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="D84" s="28" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A85" s="42">
+        <v>43251</v>
+      </c>
+      <c r="B85" s="39">
+        <v>1.5</v>
+      </c>
+      <c r="C85" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="D85" s="20" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A86" s="48"/>
+      <c r="B86" s="46"/>
+      <c r="C86" s="46"/>
+      <c r="D86" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="63">
+        <v>43251</v>
+      </c>
+      <c r="B87" s="60">
+        <v>0.5</v>
+      </c>
+      <c r="C87" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="D87" s="27" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="90.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="47">
+        <v>43252</v>
+      </c>
+      <c r="B88" s="45">
+        <v>2</v>
+      </c>
+      <c r="C88" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A89" s="43"/>
+      <c r="B89" s="40"/>
+      <c r="C89" s="40"/>
+      <c r="D89" s="30" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A90" s="48"/>
+      <c r="B90" s="46"/>
+      <c r="C90" s="46"/>
+      <c r="D90" s="8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A91" s="64">
+        <v>43252</v>
+      </c>
+      <c r="B91" s="57">
+        <v>1</v>
+      </c>
+      <c r="C91" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="D91" s="28" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A92" s="64">
+        <v>43252</v>
+      </c>
+      <c r="B92" s="57">
+        <v>1</v>
+      </c>
+      <c r="C92" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="D92" s="28" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A93" s="64">
+        <v>43252</v>
+      </c>
+      <c r="B93" s="57">
+        <v>1</v>
+      </c>
+      <c r="C93" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="D93" s="28" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="63">
+        <v>43252</v>
+      </c>
+      <c r="B94" s="60">
+        <v>0.5</v>
+      </c>
+      <c r="C94" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D94" s="27" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="53">
+  <mergeCells count="62">
+    <mergeCell ref="C88:C90"/>
+    <mergeCell ref="B88:B90"/>
+    <mergeCell ref="A88:A90"/>
+    <mergeCell ref="C81:C83"/>
+    <mergeCell ref="B81:B83"/>
+    <mergeCell ref="A81:A83"/>
+    <mergeCell ref="C85:C86"/>
+    <mergeCell ref="B85:B86"/>
+    <mergeCell ref="A85:A86"/>
+    <mergeCell ref="A68:A69"/>
+    <mergeCell ref="B68:B69"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="C65:C67"/>
+    <mergeCell ref="B65:B67"/>
+    <mergeCell ref="A65:A67"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="B52:B54"/>
+    <mergeCell ref="A52:A54"/>
+    <mergeCell ref="A55:A59"/>
+    <mergeCell ref="B55:B59"/>
+    <mergeCell ref="C55:C59"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="A44:A49"/>
+    <mergeCell ref="B44:B49"/>
+    <mergeCell ref="C44:C49"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="A14:A22"/>
+    <mergeCell ref="B14:B22"/>
+    <mergeCell ref="C14:C22"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="C36:C40"/>
+    <mergeCell ref="B36:B40"/>
+    <mergeCell ref="A36:A40"/>
     <mergeCell ref="C77:C80"/>
     <mergeCell ref="A77:A80"/>
     <mergeCell ref="B77:B80"/>
@@ -2126,50 +2399,6 @@
     <mergeCell ref="A75:A76"/>
     <mergeCell ref="B75:B76"/>
     <mergeCell ref="C75:C76"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="C36:C40"/>
-    <mergeCell ref="B36:B40"/>
-    <mergeCell ref="A36:A40"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="A14:A22"/>
-    <mergeCell ref="B14:B22"/>
-    <mergeCell ref="C14:C22"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="A44:A49"/>
-    <mergeCell ref="B44:B49"/>
-    <mergeCell ref="C44:C49"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="B52:B54"/>
-    <mergeCell ref="A52:A54"/>
-    <mergeCell ref="A55:A59"/>
-    <mergeCell ref="B55:B59"/>
-    <mergeCell ref="C55:C59"/>
-    <mergeCell ref="A68:A69"/>
-    <mergeCell ref="B68:B69"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="C65:C67"/>
-    <mergeCell ref="B65:B67"/>
-    <mergeCell ref="A65:A67"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D29" r:id="rId1"/>
@@ -2185,9 +2414,10 @@
     <hyperlink ref="D68" r:id="rId11"/>
     <hyperlink ref="D76" r:id="rId12"/>
     <hyperlink ref="D74" r:id="rId13"/>
+    <hyperlink ref="D86" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"-,Gras"Présentiel pour open space&amp;C&amp;"-,Gras"&amp;14Journal de travail&amp;R&amp;"-,Gras"Cyril Kalbfuss</oddHeader>
   </headerFooter>

</xml_diff>